<commit_message>
Analyzed Pokemon, Pokemon Species
</commit_message>
<xml_diff>
--- a/PokemonDEX.xlsx
+++ b/PokemonDEX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a994f0b6a63b5edb/Education/Drexel/2019 - 2020/Fall/DSCI 511/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Education\Drexel\2019 - 2020\Fall\DSCI 511\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{16E7CC67-397C-49EF-9C6D-FF31496E9BBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{74B23A0D-C5E0-46BF-A5FC-DF5083C275A1}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{16E7CC67-397C-49EF-9C6D-FF31496E9BBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{462994AC-18C0-4CD4-832E-0D5157A51A1E}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{190B8D52-6F1B-4018-9089-E62F6D06F5F7}"/>
+    <workbookView xWindow="34005" yWindow="3330" windowWidth="19995" windowHeight="11055" xr2:uid="{190B8D52-6F1B-4018-9089-E62F6D06F5F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Evolve to</t>
   </si>
   <si>
-    <t>Type (fire, water)</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Abilities (World ability)</t>
   </si>
   <si>
-    <t>From Game Appearances</t>
-  </si>
-  <si>
     <t># Games appearances</t>
   </si>
   <si>
@@ -126,9 +120,6 @@
     <t>Species -&gt; evolution_chain</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>height</t>
   </si>
   <si>
@@ -153,9 +144,6 @@
     <t>https://pokeapi.co/docs/v2.html/#evolution-section</t>
   </si>
   <si>
-    <t>https://pokeapi.co/docs/v2.html/#games-section</t>
-  </si>
-  <si>
     <t>Growth Rate</t>
   </si>
   <si>
@@ -168,7 +156,13 @@
     <t>https://pokeapi.co/docs/v2.html/#pokemon-shapes</t>
   </si>
   <si>
-    <t>https://pokeapi.co/docs/v2.html/#pokemon-species</t>
+    <t>species -&gt; id</t>
+  </si>
+  <si>
+    <t>species -&gt; generation</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -540,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64BD351-4CF7-413C-95C3-EC684A16329F}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,26 +558,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,79 +588,109 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -671,10 +698,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -682,26 +709,29 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,18 +739,21 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -728,23 +761,17 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -754,62 +781,57 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C16" r:id="rId1" location="evolution-section" xr:uid="{4BC787CF-49BB-418D-AA88-560A885D1523}"/>
-    <hyperlink ref="C19" r:id="rId2" location="games-section" xr:uid="{F756110B-09E5-4FD3-9A76-30729CB0843D}"/>
-    <hyperlink ref="C36" r:id="rId3" location="growth-rates" xr:uid="{88937059-BE13-478C-B10E-A7FB4AA0C971}"/>
-    <hyperlink ref="C35" r:id="rId4" xr:uid="{9153FB73-3139-4ABC-8146-A07F96DE3E1E}"/>
-    <hyperlink ref="C37" r:id="rId5" location="pokemon-shapes" xr:uid="{F3675899-B7CC-4190-9DCF-3D60BAB822E8}"/>
-    <hyperlink ref="C14" r:id="rId6" location="pokemon-species" xr:uid="{A194FC5C-2334-42BA-9B97-6A9DE90CC468}"/>
-    <hyperlink ref="C15" r:id="rId7" location="pokemon-species" xr:uid="{B03B17DF-9B08-4BC3-AE71-6BAFAA5A4711}"/>
+    <hyperlink ref="C36" r:id="rId1" location="evolution-section" xr:uid="{4BC787CF-49BB-418D-AA88-560A885D1523}"/>
+    <hyperlink ref="C34" r:id="rId2" location="growth-rates" xr:uid="{88937059-BE13-478C-B10E-A7FB4AA0C971}"/>
+    <hyperlink ref="C33" r:id="rId3" xr:uid="{9153FB73-3139-4ABC-8146-A07F96DE3E1E}"/>
+    <hyperlink ref="C35" r:id="rId4" location="pokemon-shapes" xr:uid="{F3675899-B7CC-4190-9DCF-3D60BAB822E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>